<commit_message>
Update class java follow rubric
</commit_message>
<xml_diff>
--- a/Hotel_Application_Data.xlsx
+++ b/Hotel_Application_Data.xlsx
@@ -13,9 +13,9 @@
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Customers" r:id="rId7" sheetId="28"/>
-    <sheet name="Reservations" r:id="rId8" sheetId="29"/>
-    <sheet name="Rooms" r:id="rId9" sheetId="30"/>
+    <sheet name="Customers" r:id="rId7" sheetId="31"/>
+    <sheet name="Reservations" r:id="rId8" sheetId="32"/>
+    <sheet name="Rooms" r:id="rId9" sheetId="33"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="33">
   <si>
     <t>Customer First Name</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>04/01/2024 00:51:32</t>
+  </si>
+  <si>
+    <t>quynh</t>
+  </si>
+  <si>
+    <t>quynh@domain.com</t>
   </si>
 </sst>
 </file>
@@ -478,9 +484,9 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -530,12 +536,23 @@
         <v>26</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -664,7 +681,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:D5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Fix validate room number is a number
</commit_message>
<xml_diff>
--- a/Hotel_Application_Data.xlsx
+++ b/Hotel_Application_Data.xlsx
@@ -13,9 +13,9 @@
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Customers" r:id="rId7" sheetId="31"/>
-    <sheet name="Reservations" r:id="rId8" sheetId="32"/>
-    <sheet name="Rooms" r:id="rId9" sheetId="33"/>
+    <sheet name="Customers" r:id="rId7" sheetId="46"/>
+    <sheet name="Reservations" r:id="rId8" sheetId="47"/>
+    <sheet name="Rooms" r:id="rId9" sheetId="48"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="36">
   <si>
     <t>Customer First Name</t>
   </si>
@@ -134,6 +134,15 @@
   </si>
   <si>
     <t>quynh@domain.com</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>303</t>
   </si>
 </sst>
 </file>
@@ -484,7 +493,7 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -552,7 +561,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -681,9 +690,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -759,6 +768,48 @@
         <v>15</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Update fix bug infinity loop
</commit_message>
<xml_diff>
--- a/Hotel_Application_Data.xlsx
+++ b/Hotel_Application_Data.xlsx
@@ -13,9 +13,9 @@
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Customers" r:id="rId7" sheetId="46"/>
-    <sheet name="Reservations" r:id="rId8" sheetId="47"/>
-    <sheet name="Rooms" r:id="rId9" sheetId="48"/>
+    <sheet name="Customers" r:id="rId7" sheetId="51"/>
+    <sheet name="Reservations" r:id="rId8" sheetId="52"/>
+    <sheet name="Rooms" r:id="rId9" sheetId="53"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="37">
   <si>
     <t>Customer First Name</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>303</t>
+  </si>
+  <si>
+    <t>505</t>
   </si>
 </sst>
 </file>
@@ -493,7 +496,7 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -561,7 +564,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -690,9 +693,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -810,6 +813,20 @@
         <v>19</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Add suggest checkin and checkout date
</commit_message>
<xml_diff>
--- a/Hotel_Application_Data.xlsx
+++ b/Hotel_Application_Data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/congdinh/Documents/github/congdinh2008/java-programming-udacity-prj1-hotel-reservation-application/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52165C15-9493-DC4A-8EFD-8A84AE6AE5CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FA997F-AD9D-524D-97E5-E546D5675C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="38400" windowHeight="21100" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Customers" r:id="rId7" sheetId="51"/>
-    <sheet name="Reservations" r:id="rId8" sheetId="52"/>
-    <sheet name="Rooms" r:id="rId9" sheetId="53"/>
+    <sheet name="Customers" r:id="rId9" sheetId="67"/>
+    <sheet name="Reservations" r:id="rId7" sheetId="68"/>
+    <sheet name="Rooms" r:id="rId8" sheetId="69"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="30">
   <si>
     <t>Customer First Name</t>
   </si>
@@ -85,67 +85,46 @@
     <t>No</t>
   </si>
   <si>
-    <t>102</t>
-  </si>
-  <si>
     <t>Double</t>
   </si>
   <si>
-    <t>103</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>104</t>
   </si>
   <si>
+    <t>thang</t>
+  </si>
+  <si>
+    <t>thang@domain.com</t>
+  </si>
+  <si>
+    <t>quynh</t>
+  </si>
+  <si>
+    <t>quynh@domain.com</t>
+  </si>
+  <si>
     <t>Check In Date</t>
   </si>
   <si>
     <t>Check Out Date</t>
   </si>
   <si>
-    <t>01/01/2024 16:57:09</t>
-  </si>
-  <si>
-    <t>05/01/2024 16:57:13</t>
-  </si>
-  <si>
-    <t>thang</t>
-  </si>
-  <si>
-    <t>thang@domain.com</t>
-  </si>
-  <si>
-    <t>01/01/2024 00:48:13</t>
-  </si>
-  <si>
-    <t>04/01/2024 00:48:19</t>
-  </si>
-  <si>
-    <t>01/01/2024 00:51:26</t>
-  </si>
-  <si>
-    <t>04/01/2024 00:51:32</t>
-  </si>
-  <si>
-    <t>quynh</t>
-  </si>
-  <si>
-    <t>quynh@domain.com</t>
-  </si>
-  <si>
-    <t>106</t>
-  </si>
-  <si>
-    <t>107</t>
-  </si>
-  <si>
-    <t>303</t>
-  </si>
-  <si>
-    <t>505</t>
+    <t>01/01/2024 08:48:15</t>
+  </si>
+  <si>
+    <t>01/04/2024 08:48:23</t>
+  </si>
+  <si>
+    <t>01/01/2024 08:47:15</t>
+  </si>
+  <si>
+    <t>01/04/2024 08:47:20</t>
+  </si>
+  <si>
+    <t>01/08/2024 09:00:35</t>
+  </si>
+  <si>
+    <t>01/11/2024 09:00:41</t>
   </si>
 </sst>
 </file>
@@ -496,7 +475,7 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -539,24 +518,24 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -564,7 +543,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -595,10 +574,10 @@
         <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2">
@@ -624,39 +603,39 @@
         <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E3" t="n">
         <v>300.0</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
         <v>15</v>
       </c>
       <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
         <v>27</v>
-      </c>
-      <c r="I3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4">
@@ -670,22 +649,22 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="n">
+        <v>300.0</v>
+      </c>
+      <c r="F4" t="s">
         <v>16</v>
-      </c>
-      <c r="E4" t="n">
-        <v>200.0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
       </c>
       <c r="G4" t="s">
         <v>15</v>
       </c>
       <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
         <v>29</v>
-      </c>
-      <c r="I4" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -693,9 +672,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -717,13 +696,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B2" t="n">
-        <v>120.0</v>
+        <v>300.0</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
@@ -731,99 +710,15 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B3" t="n">
-        <v>200.0</v>
+        <v>120.0</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="n">
-        <v>300.0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="n">
-        <v>33.0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" t="n">
-        <v>19.0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update code to prevent book room not in list
</commit_message>
<xml_diff>
--- a/Hotel_Application_Data.xlsx
+++ b/Hotel_Application_Data.xlsx
@@ -14,8 +14,8 @@
   </bookViews>
   <sheets>
     <sheet name="Customers" r:id="rId9" sheetId="67"/>
-    <sheet name="Reservations" r:id="rId7" sheetId="68"/>
-    <sheet name="Rooms" r:id="rId8" sheetId="69"/>
+    <sheet name="Reservations" r:id="rId7" sheetId="70"/>
+    <sheet name="Rooms" r:id="rId8" sheetId="71"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="30">
   <si>
     <t>Customer First Name</t>
   </si>
@@ -543,7 +543,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -672,7 +672,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:D3"/>
   <sheetViews>

</xml_diff>